<commit_message>
revisi import hasil ujian (lyra)
</commit_message>
<xml_diff>
--- a/PBLSEM4/public/template_hasilUjian.xlsx
+++ b/PBLSEM4/public/template_hasilUjian.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
@@ -41,19 +41,19 @@
     <t>Reading</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Status Lulus</t>
-  </si>
-  <si>
     <t>Lyra Faiqah Bilqis</t>
   </si>
   <si>
-    <t>2025-04-15</t>
+    <t>Satria Rakhmadani</t>
   </si>
   <si>
-    <t>LULUS</t>
+    <t>Dimas Wahyu</t>
+  </si>
+  <si>
+    <t>Nicholas Saputra</t>
+  </si>
+  <si>
+    <t>Mamat Alkatiri</t>
   </si>
 </sst>
 </file>
@@ -75,6 +75,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -529,19 +530,19 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -550,7 +551,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -674,8 +675,10 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -735,6 +738,13 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/customStorage/customStorage.xml><?xml version="1.0" encoding="utf-8"?>
+<customStorage xmlns="https://web.wps.cn/et/2018/main">
+  <book/>
+  <sheets/>
+</customStorage>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1022,56 +1032,101 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="16.2857142857143" customWidth="1"/>
-    <col min="2" max="2" width="14.4285714285714" customWidth="1"/>
+    <col min="1" max="1" width="26.8571428571429" customWidth="1"/>
+    <col min="2" max="2" width="17.2857142857143" customWidth="1"/>
+    <col min="6" max="6" width="13.8571428571429" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B2" s="2">
+        <v>45762</v>
+      </c>
+      <c r="C2">
+        <v>250</v>
+      </c>
+      <c r="D2">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
+      <c r="B3" s="2">
+        <v>45760</v>
+      </c>
+      <c r="C3">
+        <v>200</v>
+      </c>
+      <c r="D3">
+        <v>180</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" s="2">
+        <v>45762</v>
+      </c>
+      <c r="C4">
+        <v>300</v>
+      </c>
+      <c r="D4">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="C2">
+      <c r="B5" s="2">
+        <v>45762</v>
+      </c>
+      <c r="C5">
         <v>300</v>
       </c>
-      <c r="D2">
-        <v>300</v>
-      </c>
-      <c r="E2">
-        <v>600</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="D5">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
         <v>8</v>
+      </c>
+      <c r="B6" s="2">
+        <v>45760</v>
+      </c>
+      <c r="C6">
+        <v>200</v>
+      </c>
+      <c r="D6">
+        <v>250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>